<commit_message>
[investigation_results] Upload investigated data
</commit_message>
<xml_diff>
--- a/manual/gs/gs_Investigation_results.xlsx
+++ b/manual/gs/gs_Investigation_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Downloads/Investigation_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B256EB-B352-1244-9567-7D703BF3171D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7728C3F2-2DB6-9F46-BB64-ACF0E282D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>IP address</t>
   </si>
@@ -128,6 +128,209 @@
   </si>
   <si>
     <t>Please upload your findings to this table. There is an example row (yellow background). Use different background colour please.</t>
+  </si>
+  <si>
+    <t>195.231.166.72</t>
+  </si>
+  <si>
+    <t>195.231.128.0/17</t>
+  </si>
+  <si>
+    <t>194.28.252.65</t>
+  </si>
+  <si>
+    <t>185.129.62.63</t>
+  </si>
+  <si>
+    <t>185.129.62.0/23</t>
+  </si>
+  <si>
+    <t>185.129.62.62</t>
+  </si>
+  <si>
+    <t>212.98.122.91</t>
+  </si>
+  <si>
+    <t>212.98.64.0/18</t>
+  </si>
+  <si>
+    <t>62.107.156.12</t>
+  </si>
+  <si>
+    <t>62.107.0.0/16</t>
+  </si>
+  <si>
+    <t>5.206.194.9</t>
+  </si>
+  <si>
+    <t>5.206.192.0/21</t>
+  </si>
+  <si>
+    <t>84.238.23.220</t>
+  </si>
+  <si>
+    <t>84.238.0.0/17</t>
+  </si>
+  <si>
+    <t>84.238.43.174</t>
+  </si>
+  <si>
+    <t>212.242.70.131</t>
+  </si>
+  <si>
+    <t>217.198.208.0/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 194.28.252.0/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Styrelsen for it og laering</t>
+  </si>
+  <si>
+    <t>UPC Schweiz, 
+Fagbevaegelsens Hovedorganisation</t>
+  </si>
+  <si>
+    <t>Zencurity ApS</t>
+  </si>
+  <si>
+    <t>Cust GC Net</t>
+  </si>
+  <si>
+    <t>Norlys Digital A/S</t>
+  </si>
+  <si>
+    <t>BOLIGNET-AARHUS F.M.B.A.</t>
+  </si>
+  <si>
+    <t>Styrelsen for it og laering</t>
+  </si>
+  <si>
+    <t>Fagbevaegelsens Hovedorganisation</t>
+  </si>
+  <si>
+    <t>GlobalConnect A/S</t>
+  </si>
+  <si>
+    <t>Telia Stofa A/S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Syd Energi Bredbaand A/S</t>
+  </si>
+  <si>
+    <t>s5h.net</t>
+  </si>
+  <si>
+    <t>Abusix Mail Intelligence Blacklist, DAN TOR, DAN TOREXIT, IMP SPAM, RATS Spam, s5h.net, SPAMCOP, Spamhaus ZEN, SWINOG</t>
+  </si>
+  <si>
+    <t>Abusix Mail Intelligence Blacklist, DAN TOR, DAN TOREXIT, RATS Spam, s5h.net, SPAMCOP, Spamhaus ZEN, SWINOG, SEM BLACK, TRUNCATE, FMB BL, Efnet BL</t>
+  </si>
+  <si>
+    <t>Sorbs, Barracuda, Spamhaus, MailSpike, FMB BL , Hostkarma</t>
+  </si>
+  <si>
+    <t>s5h.net, SORBS DUHL, Spamhaus ZEN</t>
+  </si>
+  <si>
+    <t>Abusix Mail Intelligence Blacklist, Anonmails DNSBL, BACKSCATTERER, BLOCKLIST.DE, DRONE BL, INTERSERVER, MAILSPIKE BL, MAILSPIKE Z, RATS Dyna, s5h.net, SPAMCOP, Spamhaus ZEN, SWINOG, TRUNCATE, UCEPROTECTL1, UCEPROTECTL2</t>
+  </si>
+  <si>
+    <t>UCEPROTECTL3, UCEPROTECTL2, Spamhaus ZEN, SORBS SPAM, s5h.net, RATS Dyna, DRONE BL, BARRACUDA, Anonmails DNSBL</t>
+  </si>
+  <si>
+    <t>Arhus</t>
+  </si>
+  <si>
+    <t>Sønderborg, Vordingborg</t>
+  </si>
+  <si>
+    <t>Sønderborg, Rask Molle</t>
+  </si>
+  <si>
+    <t>Aarhus</t>
+  </si>
+  <si>
+    <t>AArhus</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>TOR: TOR-Contact: Henrik Kramselund TOR-Details: N:kramse02/P:9001/F:EFGHRSDV, Data Center/Web Hosting/Transit</t>
+  </si>
+  <si>
+    <t>TOR: TOR-Contact: Henrik Kramselund TOR-Details: N:kramse01/P:9001/F:EFGHRSDV,</t>
+  </si>
+  <si>
+    <t>stil.dk</t>
+  </si>
+  <si>
+    <t>ftp.catpipe.net, proxy.catpipe.net, mirrors.catpipe.net, chef.catpipe.net, ftf.net, catpipe.net</t>
+  </si>
+  <si>
+    <t>tor02.zencurity.com, tor02.zencurity.dk, belikebill.no-ip.biz, belikebill.no-ip.biz, antvirus.ddns.com.br, ufciricto.kvrddns.com, romanep2612.dyn-vpn.de, seed.nu.crypto-daio.co.uk</t>
+  </si>
+  <si>
+    <t>tor01.zencurity.com, block2.mmms.eu, spocke.direct.quickconnect.to, ping-ip.hldns.ru, seed.nu.crypto-daio.co.uk, seed.bc.crypto-daio.co.uk, ticwcisalo.kvrddns.com, 
+beferosun.kvrddns.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3e6b9c0c.rev.stofanet.dk, </t>
+  </si>
+  <si>
+    <t>5cec209.rev.sefiber.dk</t>
+  </si>
+  <si>
+    <t>84-238-23-220.ptr.bnaa.dk</t>
+  </si>
+  <si>
+    <t>84-238-43-174.ptr.bnaa.dk</t>
+  </si>
+  <si>
+    <t>spam</t>
+  </si>
+  <si>
+    <t>file referring: https://www.virustotal.com/gui/file/b836d918e9dade4a8176484e23b6063b3a04faa24ef9a6bcd3129c31a101394c</t>
+  </si>
+  <si>
+    <t>crawler, ssh bruteforce, exploit attempt, https://viz.greynoise.io/ip/185.129.62.63, https://www.virustotal.com/gui/ip-address/185.129.62.63/relations, https://www.abuseipdb.com/check/185.129.62.63, https://otx.alienvault.com/indicator/ip/185.129.62.63</t>
+  </si>
+  <si>
+    <t>crawler, ssh bruteforce, exploit attempt, https://viz.greynoise.io/ip/185.129.62.62, https://www.virustotal.com/gui/ip-address/185.129.62.62/relations, https://www.abuseipdb.com/check/185.129.62.62, https://otx.alienvault.com/indicator/ip/185.129.62.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh bruteforce, ssh worm, IoT bruteforce, BOT, https://viz.greynoise.io/ip/212.98.122.91, https://www.abuseipdb.com/check/212.98.122.91, </t>
+  </si>
+  <si>
+    <t>ssh bruteforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh bruteforce, ssh worm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh, </t>
+  </si>
+  <si>
+    <t>9001, 9030, 2200, https://search.censys.io/hosts/185.129.62.63, https://www.shodan.io/host/185.129.62.63</t>
+  </si>
+  <si>
+    <t>123, 9001, 2200, 9030</t>
+  </si>
+  <si>
+    <t>22, 80, 123, https://www.shodan.io/host/212.98.122.91, https://search.censys.io/hosts/212.98.122.91</t>
+  </si>
+  <si>
+    <t>161, https://www.shodan.io/host/62.107.156.12#161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">443, https://www.shodan.io/host/5.206.194.9, https://search.censys.io/hosts/5.206.194.9/data/table#500-UDP-IKE, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22, 8082, https://search.censys.io/hosts/84.238.23.220, https://www.shodan.io/host/84.238.23.220, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22, SSH-2.0-dropbear, </t>
   </si>
 </sst>
 </file>
@@ -137,7 +340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +365,54 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,10 +468,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -228,8 +480,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,23 +711,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:R6"/>
+  <dimension ref="A3:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="5" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="97.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="207.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="200.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="93" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="139.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
     <col min="14" max="14" width="20.5" customWidth="1"/>
@@ -622,6 +889,265 @@
         <v>34</v>
       </c>
     </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:P4"/>

</xml_diff>

<commit_message>
[gs/investigation_results] Upload investigated data
</commit_message>
<xml_diff>
--- a/manual/gs/gs_Investigation_results.xlsx
+++ b/manual/gs/gs_Investigation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7728C3F2-2DB6-9F46-BB64-ACF0E282D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A22D333-DF15-844E-9A73-3845A35514E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="165">
   <si>
     <t>IP address</t>
   </si>
@@ -173,12 +173,6 @@
   </si>
   <si>
     <t>84.238.43.174</t>
-  </si>
-  <si>
-    <t>212.242.70.131</t>
-  </si>
-  <si>
-    <t>217.198.208.0/20</t>
   </si>
   <si>
     <t xml:space="preserve"> 194.28.252.0/14</t>
@@ -221,12 +215,6 @@
     <t>s5h.net</t>
   </si>
   <si>
-    <t>Abusix Mail Intelligence Blacklist, DAN TOR, DAN TOREXIT, IMP SPAM, RATS Spam, s5h.net, SPAMCOP, Spamhaus ZEN, SWINOG</t>
-  </si>
-  <si>
-    <t>Abusix Mail Intelligence Blacklist, DAN TOR, DAN TOREXIT, RATS Spam, s5h.net, SPAMCOP, Spamhaus ZEN, SWINOG, SEM BLACK, TRUNCATE, FMB BL, Efnet BL</t>
-  </si>
-  <si>
     <t>Sorbs, Barracuda, Spamhaus, MailSpike, FMB BL , Hostkarma</t>
   </si>
   <si>
@@ -254,28 +242,12 @@
     <t>AArhus</t>
   </si>
   <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>TOR: TOR-Contact: Henrik Kramselund TOR-Details: N:kramse02/P:9001/F:EFGHRSDV, Data Center/Web Hosting/Transit</t>
-  </si>
-  <si>
-    <t>TOR: TOR-Contact: Henrik Kramselund TOR-Details: N:kramse01/P:9001/F:EFGHRSDV,</t>
-  </si>
-  <si>
     <t>stil.dk</t>
   </si>
   <si>
     <t>ftp.catpipe.net, proxy.catpipe.net, mirrors.catpipe.net, chef.catpipe.net, ftf.net, catpipe.net</t>
   </si>
   <si>
-    <t>tor02.zencurity.com, tor02.zencurity.dk, belikebill.no-ip.biz, belikebill.no-ip.biz, antvirus.ddns.com.br, ufciricto.kvrddns.com, romanep2612.dyn-vpn.de, seed.nu.crypto-daio.co.uk</t>
-  </si>
-  <si>
-    <t>tor01.zencurity.com, block2.mmms.eu, spocke.direct.quickconnect.to, ping-ip.hldns.ru, seed.nu.crypto-daio.co.uk, seed.bc.crypto-daio.co.uk, ticwcisalo.kvrddns.com, 
-beferosun.kvrddns.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">3e6b9c0c.rev.stofanet.dk, </t>
   </si>
   <si>
@@ -291,18 +263,6 @@
     <t>spam</t>
   </si>
   <si>
-    <t>file referring: https://www.virustotal.com/gui/file/b836d918e9dade4a8176484e23b6063b3a04faa24ef9a6bcd3129c31a101394c</t>
-  </si>
-  <si>
-    <t>crawler, ssh bruteforce, exploit attempt, https://viz.greynoise.io/ip/185.129.62.63, https://www.virustotal.com/gui/ip-address/185.129.62.63/relations, https://www.abuseipdb.com/check/185.129.62.63, https://otx.alienvault.com/indicator/ip/185.129.62.63</t>
-  </si>
-  <si>
-    <t>crawler, ssh bruteforce, exploit attempt, https://viz.greynoise.io/ip/185.129.62.62, https://www.virustotal.com/gui/ip-address/185.129.62.62/relations, https://www.abuseipdb.com/check/185.129.62.62, https://otx.alienvault.com/indicator/ip/185.129.62.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssh bruteforce, ssh worm, IoT bruteforce, BOT, https://viz.greynoise.io/ip/212.98.122.91, https://www.abuseipdb.com/check/212.98.122.91, </t>
-  </si>
-  <si>
     <t>ssh bruteforce</t>
   </si>
   <si>
@@ -312,15 +272,6 @@
     <t xml:space="preserve">ssh, </t>
   </si>
   <si>
-    <t>9001, 9030, 2200, https://search.censys.io/hosts/185.129.62.63, https://www.shodan.io/host/185.129.62.63</t>
-  </si>
-  <si>
-    <t>123, 9001, 2200, 9030</t>
-  </si>
-  <si>
-    <t>22, 80, 123, https://www.shodan.io/host/212.98.122.91, https://search.censys.io/hosts/212.98.122.91</t>
-  </si>
-  <si>
     <t>161, https://www.shodan.io/host/62.107.156.12#161</t>
   </si>
   <si>
@@ -331,6 +282,240 @@
   </si>
   <si>
     <t xml:space="preserve">22, SSH-2.0-dropbear, </t>
+  </si>
+  <si>
+    <t>Government, Datacenter</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>virustotal: 0, abuseipdb: 0%</t>
+  </si>
+  <si>
+    <t>1 file: trojan.crack/utorrent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh bruteforce, ssh worm, IoT bruteforce, BOT, </t>
+  </si>
+  <si>
+    <t>Data Center/Web Hosting/Transit</t>
+  </si>
+  <si>
+    <t>22, 80, 123</t>
+  </si>
+  <si>
+    <t>virustotal: -13, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>Fixed Line ISP</t>
+  </si>
+  <si>
+    <t>virustotal: , abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>185.129.61.10</t>
+  </si>
+  <si>
+    <t>185.129.61.9</t>
+  </si>
+  <si>
+    <t>185.129.61.1</t>
+  </si>
+  <si>
+    <t>185.129.61.5</t>
+  </si>
+  <si>
+    <t>185.129.61.7</t>
+  </si>
+  <si>
+    <t>185.129.61.2</t>
+  </si>
+  <si>
+    <t>185.129.61.4</t>
+  </si>
+  <si>
+    <t>185.129.61.6</t>
+  </si>
+  <si>
+    <t>Data Center/Web Hosting/Transit, TOR</t>
+  </si>
+  <si>
+    <t>SWINOG, Spamhaus ZEN, SPAMCOP, s5h.net, RATS Spam, DAN TOREXIT, DAN TOR, Abusix Mail Intelligence Blacklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tor02.zencurity.com, </t>
+  </si>
+  <si>
+    <t>91 files: trojan</t>
+  </si>
+  <si>
+    <t>36 files: trojan</t>
+  </si>
+  <si>
+    <t>&gt;1800 files: trojan</t>
+  </si>
+  <si>
+    <t>SWINOG, Spamhaus ZEN, SPAMCOP, SEM BLACK, s5h.net, RATS Spam, DAN TOREXIT, DAN TOR, Abusix Mail Intelligence Blacklist</t>
+  </si>
+  <si>
+    <t>123, 9001, 9030</t>
+  </si>
+  <si>
+    <t>TOR, web crawler, TLS/SSL crawler, SSH bruteforce, PHPMYADMIN worm, carries http referer</t>
+  </si>
+  <si>
+    <t>tor01.zencurity.com</t>
+  </si>
+  <si>
+    <t>TOR exit nodes, the most reported ones according to abuseIPDB</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>ASN</t>
+  </si>
+  <si>
+    <t>Malicious IPs</t>
+  </si>
+  <si>
+    <t>130.225.0.0/16</t>
+  </si>
+  <si>
+    <t>193.3.192.0/19</t>
+  </si>
+  <si>
+    <t>193.163.80.0/22</t>
+  </si>
+  <si>
+    <t>192.66.104.0/21</t>
+  </si>
+  <si>
+    <t>193.162.176.0/20</t>
+  </si>
+  <si>
+    <t>Danmarks Tekniske Universitet</t>
+  </si>
+  <si>
+    <t>AS1835</t>
+  </si>
+  <si>
+    <t>130.225.165.50</t>
+  </si>
+  <si>
+    <t>University/College/School</t>
+  </si>
+  <si>
+    <t>test.oek.dk, uni-noc.dk, thom1730rbs43ntc.asuscomm.com</t>
+  </si>
+  <si>
+    <t>BARRACUDA</t>
+  </si>
+  <si>
+    <t>9030, TOR http, 2200: SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16030 http, </t>
+  </si>
+  <si>
+    <t>virustotal: -46, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>virustotal: 0, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>virustotal: -3, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssh bruteforce, TLS/SSL crawler, web crawler, carries http referer, TOR, DDoS, </t>
+  </si>
+  <si>
+    <t>virustotal: -4, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>K-Net Forening</t>
+  </si>
+  <si>
+    <t>Trafikstyrelsen</t>
+  </si>
+  <si>
+    <t>Esbjerg Kommune</t>
+  </si>
+  <si>
+    <t>Styrelsen for Arbejdsmarked og Rekruttering</t>
+  </si>
+  <si>
+    <t>193.162.120.0/21</t>
+  </si>
+  <si>
+    <t>193.162.168.0/21</t>
+  </si>
+  <si>
+    <t>192.66.100.0/22</t>
+  </si>
+  <si>
+    <t>192.66.112.0/22</t>
+  </si>
+  <si>
+    <t>130.225.244.90</t>
+  </si>
+  <si>
+    <t>130.225.39.160</t>
+  </si>
+  <si>
+    <t>130.225.165.50, 130.225.244.90, 130.225.39.160</t>
+  </si>
+  <si>
+    <t>130.226.0.0/16</t>
+  </si>
+  <si>
+    <t>130.226.169.137</t>
+  </si>
+  <si>
+    <t>AS 1835</t>
+  </si>
+  <si>
+    <t>192.38.10.202</t>
+  </si>
+  <si>
+    <t>192.38.0.0/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOR, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copenhagen, Aalborg, </t>
+  </si>
+  <si>
+    <t>DAN TOR, s5h.net</t>
+  </si>
+  <si>
+    <t>dotsrc.org, uni-noc.dk, tor-relay.dotsrc.org</t>
+  </si>
+  <si>
+    <t>80: http, 161:SNMP, 443:https, 9001:https, 9030:http</t>
+  </si>
+  <si>
+    <t>682 files: trojan, ransom</t>
+  </si>
+  <si>
+    <t>22: SSH</t>
+  </si>
+  <si>
+    <t>au.dk, uni-noc.dk</t>
+  </si>
+  <si>
+    <t>DRONE BL</t>
+  </si>
+  <si>
+    <t>uni-noc.dk</t>
+  </si>
+  <si>
+    <t>9 files: trojan</t>
+  </si>
+  <si>
+    <t>Spamhaus ZEN, SORBS WEB, SORBS SPAM, BARRACUDA</t>
   </si>
 </sst>
 </file>
@@ -340,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -377,25 +562,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -404,18 +570,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="13"/>
+      <color rgb="FF20242C"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF212529"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Questrial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -470,28 +664,39 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,71 +916,71 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:R16"/>
+  <dimension ref="A3:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="207.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="200.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="222" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="208.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="93" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="139.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.5" customWidth="1"/>
     <col min="15" max="15" width="16.6640625" customWidth="1"/>
     <col min="16" max="16" width="49" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" customWidth="1"/>
+    <col min="17" max="17" width="65.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -889,269 +1094,753 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="D14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="I8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="J19" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="C22" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
         <v>99</v>
       </c>
-      <c r="K12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
         <v>100</v>
       </c>
-      <c r="K13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" s="14" t="s">
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="K14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="14" t="s">
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
         <v>102</v>
       </c>
-      <c r="K15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C46" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:P4"/>
+    <mergeCell ref="C22:C29"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1" display="https://apps.db.ripe.net/db-web-ui/lookup?source=ripe&amp;key=192.38.0.0%2F17AS1835&amp;type=route" xr:uid="{71F26DE2-A142-3646-A73E-E5502480F7EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D32" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[gs/investigation_results] Add more information.
</commit_message>
<xml_diff>
--- a/manual/gs/gs_Investigation_results.xlsx
+++ b/manual/gs/gs_Investigation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A22D333-DF15-844E-9A73-3845A35514E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FB24F8-3E2A-0C45-9EFE-58436B759833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="172">
   <si>
     <t>IP address</t>
   </si>
@@ -272,15 +272,6 @@
     <t xml:space="preserve">ssh, </t>
   </si>
   <si>
-    <t>161, https://www.shodan.io/host/62.107.156.12#161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">443, https://www.shodan.io/host/5.206.194.9, https://search.censys.io/hosts/5.206.194.9/data/table#500-UDP-IKE, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22, 8082, https://search.censys.io/hosts/84.238.23.220, https://www.shodan.io/host/84.238.23.220, </t>
-  </si>
-  <si>
     <t xml:space="preserve">22, SSH-2.0-dropbear, </t>
   </si>
   <si>
@@ -302,9 +293,6 @@
     <t>Data Center/Web Hosting/Transit</t>
   </si>
   <si>
-    <t>22, 80, 123</t>
-  </si>
-  <si>
     <t>virustotal: -13, abuseipdb: 100%</t>
   </si>
   <si>
@@ -359,18 +347,12 @@
     <t>SWINOG, Spamhaus ZEN, SPAMCOP, SEM BLACK, s5h.net, RATS Spam, DAN TOREXIT, DAN TOR, Abusix Mail Intelligence Blacklist</t>
   </si>
   <si>
-    <t>123, 9001, 9030</t>
-  </si>
-  <si>
     <t>TOR, web crawler, TLS/SSL crawler, SSH bruteforce, PHPMYADMIN worm, carries http referer</t>
   </si>
   <si>
     <t>tor01.zencurity.com</t>
   </si>
   <si>
-    <t>TOR exit nodes, the most reported ones according to abuseIPDB</t>
-  </si>
-  <si>
     <t>Network</t>
   </si>
   <si>
@@ -434,9 +416,6 @@
     <t>virustotal: -4, abuseipdb: 100%</t>
   </si>
   <si>
-    <t>K-Net Forening</t>
-  </si>
-  <si>
     <t>Trafikstyrelsen</t>
   </si>
   <si>
@@ -516,6 +495,48 @@
   </si>
   <si>
     <t>Spamhaus ZEN, SORBS WEB, SORBS SPAM, BARRACUDA</t>
+  </si>
+  <si>
+    <t>dnsbl.justspam.org</t>
+  </si>
+  <si>
+    <t>Aalborg</t>
+  </si>
+  <si>
+    <t>Danmarks Tekniske Universitet, Net til Kennedy-kollegiet</t>
+  </si>
+  <si>
+    <t>Forskningsnettet - danish network for research and education</t>
+  </si>
+  <si>
+    <t>TOR exit nodes, the most reported ones according to abuseIPDB, reported in several category but we can't distinguis between the owner and the malicious actor.</t>
+  </si>
+  <si>
+    <t>AS5624</t>
+  </si>
+  <si>
+    <t>123: NTP, 9001: https , 9030: tor http</t>
+  </si>
+  <si>
+    <t>22: ssh dropbear, 8082: http</t>
+  </si>
+  <si>
+    <t>443: https, 500: IKE</t>
+  </si>
+  <si>
+    <t>161: snmp</t>
+  </si>
+  <si>
+    <t>22: ssh, 80: http apache, 123: ntp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danmarks Tekniske Universitet, Aalborg Universitet, </t>
+  </si>
+  <si>
+    <t>Open HTTP proxy</t>
+  </si>
+  <si>
+    <t>Spam</t>
   </si>
 </sst>
 </file>
@@ -666,22 +687,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -690,12 +703,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -918,8 +938,8 @@
   </sheetPr>
   <dimension ref="A3:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -927,7 +947,7 @@
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="222" bestFit="1" customWidth="1"/>
@@ -945,42 +965,42 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1095,739 +1115,752 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="11" t="s">
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="J9" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="G14" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11" t="s">
+      <c r="G15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="11" t="s">
+      <c r="L15" s="7"/>
+      <c r="M15" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="J19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="J16" s="11" t="s">
+      <c r="C20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="K16" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>115</v>
+        <v>93</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="10"/>
+        <v>95</v>
+      </c>
+      <c r="C24" s="18"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>96</v>
+      </c>
+      <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="10"/>
+        <v>97</v>
+      </c>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>98</v>
+      </c>
+      <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="10"/>
+        <v>99</v>
+      </c>
+      <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="10"/>
+        <v>100</v>
+      </c>
+      <c r="C29" s="18"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>149</v>
+        <v>118</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>124</v>
+      <c r="C33" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="14"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E35" s="14"/>
+        <v>131</v>
+      </c>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="14"/>
+        <v>133</v>
+      </c>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C46" s="14"/>
+      <c r="C46" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
[investigation] Add new infos
</commit_message>
<xml_diff>
--- a/manual/gs/gs_Investigation_results.xlsx
+++ b/manual/gs/gs_Investigation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBFA921-FF87-E047-8B7B-8C0C75E978A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980743A0-1973-0B46-B736-7500EE4D15E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="260">
   <si>
     <t>IP address</t>
   </si>
@@ -842,6 +842,9 @@
   </si>
   <si>
     <t>So basically Zencuity is a one man stand company, maintaining an ASN. The malicious IPs are part of that ASN, and right now seems like to assigned to a dotsrc project, which is providing tor nodes on these addresses. Other than that the other Zencurity IP addresses are also tor nodes, however seems like not part of the dotsrc poject. The owner of this company is a cyber security specialist, with github repo, teaching at a Danish IT school as well.</t>
+  </si>
+  <si>
+    <t>The most reported Tor IP addresses belong to an organization called Zencurity Aps, which is a one employee company. The owner (and the only employee as well) is a cybersecurity porfessional, who is teaching cyber security at KEA education center. Through this company he is lending IP addresses to dotsrc, which is a smaller research company wit a Tor project. The project is sponsored by Aalborg University as well. The Zencurity Aps has it's own IP addresses for Tor projects as well.</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1012,15 +1015,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1242,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1269,7 +1278,7 @@
     <col min="22" max="22" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="56" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>191</v>
       </c>
@@ -1282,7 +1291,7 @@
       <c r="D1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="16" t="s">
         <v>258</v>
       </c>
     </row>
@@ -1299,7 +1308,7 @@
       <c r="D2" t="s">
         <v>199</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -1313,7 +1322,10 @@
       <c r="D3" t="s">
         <v>200</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="E3" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="V3" s="10" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1330,7 +1342,8 @@
       <c r="D4" t="s">
         <v>201</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="E4" s="17"/>
+      <c r="V4" s="11" t="s">
         <v>211</v>
       </c>
     </row>
@@ -1341,10 +1354,11 @@
       <c r="B5" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="E5" s="17"/>
+      <c r="V5" s="11" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1358,7 +1372,8 @@
       <c r="D6" t="s">
         <v>203</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="E6" s="17"/>
+      <c r="V6" s="11" t="s">
         <v>213</v>
       </c>
     </row>
@@ -1372,7 +1387,8 @@
       <c r="D7" t="s">
         <v>204</v>
       </c>
-      <c r="V7" s="14" t="s">
+      <c r="E7" s="17"/>
+      <c r="V7" s="11" t="s">
         <v>214</v>
       </c>
     </row>
@@ -1386,7 +1402,7 @@
       <c r="D8" t="s">
         <v>205</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="V8" s="11" t="s">
         <v>215</v>
       </c>
     </row>
@@ -1400,7 +1416,7 @@
       <c r="D9" t="s">
         <v>206</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="V9" s="11" t="s">
         <v>216</v>
       </c>
     </row>
@@ -1411,10 +1427,10 @@
       <c r="B10" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="11" t="s">
         <v>217</v>
       </c>
     </row>
@@ -1425,61 +1441,61 @@
       <c r="B11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="V11" s="14" t="s">
+      <c r="V11" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V12" s="14" t="s">
+      <c r="V12" s="11" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V13" s="14" t="s">
+      <c r="V13" s="11" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="V14" s="14" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="V14" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="V15" s="14" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="V15" s="11" t="s">
         <v>222</v>
       </c>
     </row>
@@ -1538,7 +1554,7 @@
       <c r="R16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V16" s="14" t="s">
+      <c r="V16" s="11" t="s">
         <v>223</v>
       </c>
     </row>
@@ -1597,7 +1613,7 @@
       <c r="R17" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="V17" s="11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -1656,7 +1672,7 @@
       <c r="R18" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V18" s="14" t="s">
+      <c r="V18" s="11" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1715,7 +1731,7 @@
       <c r="R19" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V19" s="14" t="s">
+      <c r="V19" s="11" t="s">
         <v>226</v>
       </c>
     </row>
@@ -1774,7 +1790,7 @@
       <c r="R20" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V20" s="14" t="s">
+      <c r="V20" s="11" t="s">
         <v>227</v>
       </c>
     </row>
@@ -1833,7 +1849,7 @@
       <c r="R21" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V21" s="14" t="s">
+      <c r="V21" s="11" t="s">
         <v>228</v>
       </c>
     </row>
@@ -1892,7 +1908,7 @@
       <c r="R22" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V22" s="14" t="s">
+      <c r="V22" s="11" t="s">
         <v>229</v>
       </c>
     </row>
@@ -1951,7 +1967,7 @@
       <c r="R23" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="V23" s="11" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2010,7 +2026,7 @@
       <c r="R24" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V24" s="14" t="s">
+      <c r="V24" s="11" t="s">
         <v>231</v>
       </c>
     </row>
@@ -2069,7 +2085,7 @@
       <c r="R25" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V25" s="14" t="s">
+      <c r="V25" s="11" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2128,7 +2144,7 @@
       <c r="R26" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="V26" s="11" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2187,7 +2203,7 @@
       <c r="R27" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V27" s="14" t="s">
+      <c r="V27" s="11" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2246,7 +2262,7 @@
       <c r="R28" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V28" s="14" t="s">
+      <c r="V28" s="11" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2305,7 +2321,7 @@
       <c r="R29" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V29" s="14" t="s">
+      <c r="V29" s="11" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2364,7 +2380,7 @@
       <c r="R30" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V30" s="14" t="s">
+      <c r="V30" s="11" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2423,7 +2439,7 @@
       <c r="R31" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V31" s="14" t="s">
+      <c r="V31" s="11" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2446,7 +2462,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
-      <c r="V32" s="14" t="s">
+      <c r="V32" s="11" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2455,7 +2471,7 @@
       <c r="B33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="15" t="s">
         <v>156</v>
       </c>
       <c r="D33" s="6"/>
@@ -2473,7 +2489,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
-      <c r="V33" s="14" t="s">
+      <c r="V33" s="11" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2482,7 +2498,7 @@
       <c r="B34" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2498,7 +2514,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
-      <c r="V34" s="14" t="s">
+      <c r="V34" s="11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2507,7 +2523,7 @@
       <c r="B35" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2523,7 +2539,7 @@
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
-      <c r="V35" s="14" t="s">
+      <c r="V35" s="11" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2532,7 +2548,7 @@
       <c r="B36" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -2548,7 +2564,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
-      <c r="V36" s="14" t="s">
+      <c r="V36" s="11" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2557,7 +2573,7 @@
       <c r="B37" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -2573,7 +2589,7 @@
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
-      <c r="V37" s="14" t="s">
+      <c r="V37" s="11" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2582,7 +2598,7 @@
       <c r="B38" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -2598,7 +2614,7 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
-      <c r="V38" s="14" t="s">
+      <c r="V38" s="11" t="s">
         <v>245</v>
       </c>
     </row>
@@ -2607,7 +2623,7 @@
       <c r="B39" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2623,7 +2639,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
-      <c r="V39" s="14" t="s">
+      <c r="V39" s="11" t="s">
         <v>246</v>
       </c>
     </row>
@@ -2632,7 +2648,7 @@
       <c r="B40" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -2682,7 +2698,7 @@
       <c r="D42" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="V42" s="15" t="s">
+      <c r="V42" s="12" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2699,7 +2715,7 @@
       <c r="D43" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="V43" s="12" t="s">
+      <c r="V43" s="9" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2717,7 +2733,7 @@
         <v>135</v>
       </c>
       <c r="E44" s="7"/>
-      <c r="V44" s="13" t="s">
+      <c r="V44" s="10" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2735,7 +2751,7 @@
         <v>181</v>
       </c>
       <c r="E45" s="5"/>
-      <c r="V45" s="14" t="s">
+      <c r="V45" s="11" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2753,7 +2769,7 @@
         <v>181</v>
       </c>
       <c r="E46" s="7"/>
-      <c r="V46" s="14" t="s">
+      <c r="V46" s="11" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2771,7 +2787,7 @@
         <v>181</v>
       </c>
       <c r="E47" s="7"/>
-      <c r="V47" s="14" t="s">
+      <c r="V47" s="11" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2788,7 +2804,7 @@
       <c r="D48" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V48" s="14" t="s">
+      <c r="V48" s="11" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2805,7 +2821,7 @@
       <c r="D49" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V49" s="14" t="s">
+      <c r="V49" s="11" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2822,7 +2838,7 @@
       <c r="D50" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V50" s="14" t="s">
+      <c r="V50" s="11" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2839,7 +2855,7 @@
       <c r="D51" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V51" s="14" t="s">
+      <c r="V51" s="11" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2856,260 +2872,261 @@
       <c r="D52" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V52" s="14" t="s">
+      <c r="V52" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V53" s="14" t="s">
+      <c r="V53" s="11" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V54" s="14" t="s">
+      <c r="V54" s="11" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V55" s="14" t="s">
+      <c r="V55" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V56" s="14" t="s">
+      <c r="V56" s="11" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C57" s="7"/>
-      <c r="V57" s="14" t="s">
+      <c r="V57" s="11" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V58" s="14" t="s">
+      <c r="V58" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V59" s="14" t="s">
+      <c r="V59" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V60" s="14" t="s">
+      <c r="V60" s="11" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V61" s="14" t="s">
+      <c r="V61" s="11" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V62" s="14" t="s">
+      <c r="V62" s="11" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V63" s="14" t="s">
+      <c r="V63" s="11" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V64" s="14" t="s">
+      <c r="V64" s="11" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="65" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V65" s="14" t="s">
+      <c r="V65" s="11" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="66" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V66" s="14" t="s">
+      <c r="V66" s="11" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="67" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V67" s="14" t="s">
+      <c r="V67" s="11" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="68" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V68" s="14" t="s">
+      <c r="V68" s="11" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="69" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V69" s="14" t="s">
+      <c r="V69" s="11" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="70" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V70" s="14" t="s">
+      <c r="V70" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="71" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V71" s="14" t="s">
+      <c r="V71" s="11" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="72" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V72" s="14" t="s">
+      <c r="V72" s="11" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="73" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V73" s="14" t="s">
+      <c r="V73" s="11" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="74" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V74" s="14" t="s">
+      <c r="V74" s="11" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="75" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V75" s="14" t="s">
+      <c r="V75" s="11" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="76" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V76" s="14" t="s">
+      <c r="V76" s="11" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="77" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V77" s="14" t="s">
+      <c r="V77" s="11" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="78" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V78" s="14" t="s">
+      <c r="V78" s="11" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="79" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V79" s="14" t="s">
+      <c r="V79" s="11" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="80" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V80" s="14" t="s">
+      <c r="V80" s="11" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="81" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V81" s="14" t="s">
+      <c r="V81" s="11" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="82" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V82" s="14" t="s">
+      <c r="V82" s="11" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="83" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V83" s="14" t="s">
+      <c r="V83" s="11" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="84" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V84" s="14" t="s">
+      <c r="V84" s="11" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="87" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V87" s="14" t="s">
+      <c r="V87" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="88" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V88" s="13" t="s">
+      <c r="V88" s="10" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="89" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V89" s="14" t="s">
+      <c r="V89" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="90" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V90" s="14" t="s">
+      <c r="V90" s="11" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="91" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V91" s="14" t="s">
+      <c r="V91" s="11" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="92" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V92" s="14" t="s">
+      <c r="V92" s="11" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="93" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V93" s="14" t="s">
+      <c r="V93" s="11" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="94" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V94" s="14" t="s">
+      <c r="V94" s="11" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="95" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V95" s="14" t="s">
+      <c r="V95" s="11" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="96" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V96" s="14" t="s">
+      <c r="V96" s="11" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="97" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V97" s="14" t="s">
+      <c r="V97" s="11" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="98" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V98" s="14" t="s">
+      <c r="V98" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="99" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V99" s="14" t="s">
+      <c r="V99" s="11" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="100" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V100" s="14" t="s">
+      <c r="V100" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="101" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V101" s="14" t="s">
+      <c r="V101" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="102" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V102" s="14" t="s">
+      <c r="V102" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="103" spans="22:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="V103" s="14" t="s">
+      <c r="V103" s="11" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A14:P15"/>
     <mergeCell ref="C33:C40"/>
+    <mergeCell ref="E3:E7"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3206,6 +3223,8 @@
     <hyperlink ref="V101" r:id="rId91" display="https://www.domainiq.com/domain?vikingscan.org" xr:uid="{B52946EC-6B5B-A549-9C45-CB9D09E702DF}"/>
     <hyperlink ref="V102" r:id="rId92" display="https://www.domainiq.com/domain?zencurity.org" xr:uid="{D2047129-E722-534B-8409-5DF1C2EF98A1}"/>
     <hyperlink ref="V103" r:id="rId93" display="https://www.domainiq.com/domain?kramse.surf" xr:uid="{061238B5-DD8A-204F-9229-167DECAF4531}"/>
+    <hyperlink ref="D10" r:id="rId94" xr:uid="{A8BE9B15-9F75-304F-A775-BED05E612CD2}"/>
+    <hyperlink ref="D5" r:id="rId95" xr:uid="{8E6C4CA4-BE0F-3443-93DE-07DBB6C785E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
[gs/] Add .txt with the ip-asn pairs.
</commit_message>
<xml_diff>
--- a/manual/gs/gs_Investigation_results.xlsx
+++ b/manual/gs/gs_Investigation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/gs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980743A0-1973-0B46-B736-7500EE4D15E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B80569C-3CDD-7C4C-BC91-27B6A7AADE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,13 +1019,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:V103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1291,7 +1291,7 @@
       <c r="D1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>258</v>
       </c>
     </row>
@@ -1456,45 +1456,45 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
       <c r="V14" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
       <c r="V15" s="11" t="s">
         <v>222</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="B33" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>156</v>
       </c>
       <c r="D33" s="6"/>
@@ -2498,7 +2498,7 @@
       <c r="B34" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -2523,7 +2523,7 @@
       <c r="B35" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2548,7 +2548,7 @@
       <c r="B36" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -2573,7 +2573,7 @@
       <c r="B37" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -2598,7 +2598,7 @@
       <c r="B38" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -2623,7 +2623,7 @@
       <c r="B39" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="15"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -2648,7 +2648,7 @@
       <c r="B40" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>

</xml_diff>